<commit_message>
For full test run
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_JOB_2020.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_JOB_2020.xlsx
@@ -549,7 +549,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="B:B C23"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="B:B A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -824,7 +824,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="B:B A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -878,7 +878,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="B:B G34"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -926,7 +926,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="1" sqref="B:B G15"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1295,15 +1295,15 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>42</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>46</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>47</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>48</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>50</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>51</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>52</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>53</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>56</v>
       </c>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="1" sqref="B:B G33"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1442,7 +1442,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="B:B A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1853,7 +1853,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="B:B A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>